<commit_message>
removed nested lists, used combined lists
</commit_message>
<xml_diff>
--- a/221216-RegularFaculty.xlsx
+++ b/221216-RegularFaculty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/depts/MIO/MIO Co-op/Special Projects/TTS Faculty Sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wjx\Desktop\Website Scraper\TTS-Faculty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50A8A18-A6C4-A941-A099-3897A317281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EB0ED6-2D0E-472F-A5BE-151B9E316403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19440" yWindow="540" windowWidth="18020" windowHeight="18600" xr2:uid="{40562DC0-C0B9-4750-98A8-123A25649F57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40562DC0-C0B9-4750-98A8-123A25649F57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="343">
   <si>
     <t>Statistics and Actuarial Science</t>
   </si>
@@ -1074,16 +1074,24 @@
   </si>
   <si>
     <t>Grace Yi</t>
+  </si>
+  <si>
+    <t>BIOL, CHEMENG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1106,8 +1114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7024,7 +7033,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7312,7 +7321,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7322,19 +7331,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D76A832-B0A3-4111-9115-F50C448159B4}">
   <dimension ref="A1:D309"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:D76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -7348,7 +7357,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>263</v>
       </c>
@@ -7359,7 +7368,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>270</v>
       </c>
@@ -7370,7 +7379,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -7381,7 +7390,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>258</v>
       </c>
@@ -7392,7 +7401,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>255</v>
       </c>
@@ -7406,7 +7415,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>260</v>
       </c>
@@ -7417,7 +7426,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -7428,7 +7437,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -7439,7 +7448,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>265</v>
       </c>
@@ -7453,7 +7462,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>272</v>
       </c>
@@ -7464,7 +7473,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>262</v>
       </c>
@@ -7475,7 +7484,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>256</v>
       </c>
@@ -7486,7 +7495,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>274</v>
       </c>
@@ -7497,7 +7506,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>275</v>
       </c>
@@ -7508,7 +7517,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>254</v>
       </c>
@@ -7519,7 +7528,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>249</v>
       </c>
@@ -7533,7 +7542,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>281</v>
       </c>
@@ -7543,11 +7552,11 @@
       <c r="C18" t="s">
         <v>247</v>
       </c>
-      <c r="D18" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D18" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>273</v>
       </c>
@@ -7558,7 +7567,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>271</v>
       </c>
@@ -7569,7 +7578,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>261</v>
       </c>
@@ -7583,7 +7592,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>264</v>
       </c>
@@ -7594,7 +7603,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>248</v>
       </c>
@@ -7605,7 +7614,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -7616,7 +7625,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>250</v>
       </c>
@@ -7627,7 +7636,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>268</v>
       </c>
@@ -7638,7 +7647,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>251</v>
       </c>
@@ -7649,7 +7658,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>259</v>
       </c>
@@ -7660,7 +7669,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>267</v>
       </c>
@@ -7671,7 +7680,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>269</v>
       </c>
@@ -7682,7 +7691,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -7693,7 +7702,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -7704,7 +7713,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -7715,7 +7724,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>246</v>
       </c>
@@ -7726,7 +7735,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>233</v>
       </c>
@@ -7737,7 +7746,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>235</v>
       </c>
@@ -7748,7 +7757,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>243</v>
       </c>
@@ -7759,7 +7768,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>240</v>
       </c>
@@ -7770,7 +7779,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -7781,7 +7790,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>242</v>
       </c>
@@ -7792,7 +7801,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>232</v>
       </c>
@@ -7803,7 +7812,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>241</v>
       </c>
@@ -7814,7 +7823,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>234</v>
       </c>
@@ -7825,7 +7834,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>239</v>
       </c>
@@ -7836,7 +7845,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>236</v>
       </c>
@@ -7847,7 +7856,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>245</v>
       </c>
@@ -7858,7 +7867,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>238</v>
       </c>
@@ -7869,7 +7878,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>282</v>
       </c>
@@ -7880,7 +7889,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>124</v>
       </c>
@@ -7891,7 +7900,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>162</v>
       </c>
@@ -7902,7 +7911,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>187</v>
       </c>
@@ -7913,7 +7922,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -7924,7 +7933,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>195</v>
       </c>
@@ -7935,7 +7944,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>197</v>
       </c>
@@ -7946,7 +7955,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -7957,7 +7966,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>192</v>
       </c>
@@ -7968,7 +7977,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>164</v>
       </c>
@@ -7979,7 +7988,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -7990,7 +7999,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>129</v>
       </c>
@@ -8001,7 +8010,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>291</v>
       </c>
@@ -8012,7 +8021,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>116</v>
       </c>
@@ -8023,7 +8032,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>171</v>
       </c>
@@ -8034,7 +8043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -8045,7 +8054,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -8056,7 +8065,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>196</v>
       </c>
@@ -8067,7 +8076,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -8078,7 +8087,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>161</v>
       </c>
@@ -8089,7 +8098,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>191</v>
       </c>
@@ -8100,7 +8109,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>186</v>
       </c>
@@ -8111,7 +8120,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -8122,7 +8131,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -8133,7 +8142,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>108</v>
       </c>
@@ -8144,7 +8153,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -8155,7 +8164,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>288</v>
       </c>
@@ -8166,7 +8175,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>127</v>
       </c>
@@ -8177,7 +8186,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>295</v>
       </c>
@@ -8191,7 +8200,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -8202,7 +8211,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>137</v>
       </c>
@@ -8213,7 +8222,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -8224,7 +8233,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -8235,7 +8244,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -8246,7 +8255,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>122</v>
       </c>
@@ -8257,7 +8266,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>294</v>
       </c>
@@ -8268,7 +8277,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -8279,7 +8288,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>194</v>
       </c>
@@ -8290,7 +8299,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>152</v>
       </c>
@@ -8301,7 +8310,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>296</v>
       </c>
@@ -8312,7 +8321,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>125</v>
       </c>
@@ -8323,7 +8332,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>135</v>
       </c>
@@ -8334,7 +8343,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>130</v>
       </c>
@@ -8345,7 +8354,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>193</v>
       </c>
@@ -8356,7 +8365,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>147</v>
       </c>
@@ -8367,7 +8376,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>114</v>
       </c>
@@ -8378,7 +8387,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -8389,7 +8398,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>132</v>
       </c>
@@ -8400,7 +8409,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>170</v>
       </c>
@@ -8411,7 +8420,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>149</v>
       </c>
@@ -8422,7 +8431,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>126</v>
       </c>
@@ -8433,7 +8442,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>166</v>
       </c>
@@ -8444,7 +8453,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>148</v>
       </c>
@@ -8455,7 +8464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>188</v>
       </c>
@@ -8466,7 +8475,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -8477,7 +8486,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -8488,7 +8497,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>163</v>
       </c>
@@ -8499,7 +8508,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>144</v>
       </c>
@@ -8510,7 +8519,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>136</v>
       </c>
@@ -8521,7 +8530,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>134</v>
       </c>
@@ -8532,7 +8541,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>184</v>
       </c>
@@ -8543,7 +8552,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>176</v>
       </c>
@@ -8554,7 +8563,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>150</v>
       </c>
@@ -8565,7 +8574,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>121</v>
       </c>
@@ -8576,7 +8585,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -8587,7 +8596,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>299</v>
       </c>
@@ -8598,7 +8607,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>159</v>
       </c>
@@ -8609,7 +8618,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>292</v>
       </c>
@@ -8620,7 +8629,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>172</v>
       </c>
@@ -8634,7 +8643,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>165</v>
       </c>
@@ -8645,7 +8654,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>155</v>
       </c>
@@ -8656,7 +8665,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -8667,7 +8676,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>300</v>
       </c>
@@ -8678,7 +8687,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>287</v>
       </c>
@@ -8689,7 +8698,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>156</v>
       </c>
@@ -8700,7 +8709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -8711,7 +8720,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>298</v>
       </c>
@@ -8722,7 +8731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>297</v>
       </c>
@@ -8733,7 +8742,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>293</v>
       </c>
@@ -8744,7 +8753,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>128</v>
       </c>
@@ -8755,7 +8764,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>112</v>
       </c>
@@ -8766,7 +8775,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>189</v>
       </c>
@@ -8777,7 +8786,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>289</v>
       </c>
@@ -8791,7 +8800,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>290</v>
       </c>
@@ -8805,7 +8814,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>105</v>
       </c>
@@ -8816,7 +8825,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>151</v>
       </c>
@@ -8827,7 +8836,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>106</v>
       </c>
@@ -8838,7 +8847,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>118</v>
       </c>
@@ -8849,7 +8858,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>141</v>
       </c>
@@ -8860,7 +8869,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>117</v>
       </c>
@@ -8871,7 +8880,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>139</v>
       </c>
@@ -8882,7 +8891,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>110</v>
       </c>
@@ -8893,7 +8902,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>190</v>
       </c>
@@ -8904,7 +8913,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>178</v>
       </c>
@@ -8915,7 +8924,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>109</v>
       </c>
@@ -8926,7 +8935,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>145</v>
       </c>
@@ -8940,7 +8949,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>173</v>
       </c>
@@ -8951,7 +8960,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -8962,7 +8971,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>177</v>
       </c>
@@ -8973,7 +8982,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>158</v>
       </c>
@@ -8984,7 +8993,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>157</v>
       </c>
@@ -8995,7 +9004,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>182</v>
       </c>
@@ -9009,7 +9018,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>123</v>
       </c>
@@ -9023,7 +9032,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>185</v>
       </c>
@@ -9034,7 +9043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>142</v>
       </c>
@@ -9045,7 +9054,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>181</v>
       </c>
@@ -9056,7 +9065,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -9067,7 +9076,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>175</v>
       </c>
@@ -9078,7 +9087,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>111</v>
       </c>
@@ -9089,7 +9098,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>200</v>
       </c>
@@ -9100,7 +9109,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>216</v>
       </c>
@@ -9111,7 +9120,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>217</v>
       </c>
@@ -9122,7 +9131,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>202</v>
       </c>
@@ -9133,7 +9142,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>214</v>
       </c>
@@ -9144,7 +9153,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>221</v>
       </c>
@@ -9155,7 +9164,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>204</v>
       </c>
@@ -9166,7 +9175,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>227</v>
       </c>
@@ -9177,7 +9186,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>208</v>
       </c>
@@ -9188,7 +9197,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>212</v>
       </c>
@@ -9199,7 +9208,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>211</v>
       </c>
@@ -9210,7 +9219,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>223</v>
       </c>
@@ -9224,7 +9233,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>230</v>
       </c>
@@ -9235,7 +9244,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>220</v>
       </c>
@@ -9246,7 +9255,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>219</v>
       </c>
@@ -9257,7 +9266,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>218</v>
       </c>
@@ -9268,7 +9277,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>205</v>
       </c>
@@ -9282,7 +9291,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>210</v>
       </c>
@@ -9293,7 +9302,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>209</v>
       </c>
@@ -9304,7 +9313,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>224</v>
       </c>
@@ -9315,7 +9324,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>203</v>
       </c>
@@ -9329,7 +9338,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>228</v>
       </c>
@@ -9340,7 +9349,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>201</v>
       </c>
@@ -9351,7 +9360,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>229</v>
       </c>
@@ -9365,7 +9374,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>213</v>
       </c>
@@ -9376,7 +9385,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>286</v>
       </c>
@@ -9390,7 +9399,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>222</v>
       </c>
@@ -9401,7 +9410,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>284</v>
       </c>
@@ -9415,7 +9424,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>225</v>
       </c>
@@ -9426,7 +9435,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>207</v>
       </c>
@@ -9440,7 +9449,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -9451,7 +9460,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>215</v>
       </c>
@@ -9462,7 +9471,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>226</v>
       </c>
@@ -9476,7 +9485,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>285</v>
       </c>
@@ -9487,7 +9496,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>32</v>
       </c>
@@ -9498,7 +9507,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>98</v>
       </c>
@@ -9509,7 +9518,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>102</v>
       </c>
@@ -9520,7 +9529,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>103</v>
       </c>
@@ -9531,7 +9540,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>101</v>
       </c>
@@ -9542,7 +9551,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>97</v>
       </c>
@@ -9553,7 +9562,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>100</v>
       </c>
@@ -9564,7 +9573,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>244</v>
       </c>
@@ -9575,7 +9584,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>92</v>
       </c>
@@ -9586,7 +9595,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>85</v>
       </c>
@@ -9597,7 +9606,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>301</v>
       </c>
@@ -9608,7 +9617,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>84</v>
       </c>
@@ -9619,7 +9628,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>93</v>
       </c>
@@ -9630,7 +9639,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>87</v>
       </c>
@@ -9641,7 +9650,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>94</v>
       </c>
@@ -9652,7 +9661,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>91</v>
       </c>
@@ -9663,7 +9672,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>86</v>
       </c>
@@ -9674,7 +9683,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>90</v>
       </c>
@@ -9685,7 +9694,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>89</v>
       </c>
@@ -9696,7 +9705,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>95</v>
       </c>
@@ -9707,7 +9716,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>88</v>
       </c>
@@ -9718,7 +9727,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>82</v>
       </c>
@@ -9729,7 +9738,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>310</v>
       </c>
@@ -9740,7 +9749,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>79</v>
       </c>
@@ -9751,7 +9760,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>76</v>
       </c>
@@ -9762,7 +9771,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>303</v>
       </c>
@@ -9773,7 +9782,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>78</v>
       </c>
@@ -9787,7 +9796,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>64</v>
       </c>
@@ -9798,7 +9807,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>73</v>
       </c>
@@ -9809,7 +9818,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>80</v>
       </c>
@@ -9820,7 +9829,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>309</v>
       </c>
@@ -9831,7 +9840,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>75</v>
       </c>
@@ -9842,7 +9851,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>81</v>
       </c>
@@ -9853,7 +9862,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>65</v>
       </c>
@@ -9864,7 +9873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>70</v>
       </c>
@@ -9875,7 +9884,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>71</v>
       </c>
@@ -9886,7 +9895,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>307</v>
       </c>
@@ -9897,7 +9906,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>74</v>
       </c>
@@ -9908,7 +9917,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>306</v>
       </c>
@@ -9919,7 +9928,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>77</v>
       </c>
@@ -9930,7 +9939,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>68</v>
       </c>
@@ -9941,7 +9950,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>304</v>
       </c>
@@ -9952,7 +9961,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>308</v>
       </c>
@@ -9963,7 +9972,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>67</v>
       </c>
@@ -9974,7 +9983,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>72</v>
       </c>
@@ -9985,7 +9994,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>305</v>
       </c>
@@ -9996,7 +10005,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>69</v>
       </c>
@@ -10007,7 +10016,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>302</v>
       </c>
@@ -10018,7 +10027,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>66</v>
       </c>
@@ -10029,7 +10038,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>62</v>
       </c>
@@ -10040,7 +10049,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>63</v>
       </c>
@@ -10051,7 +10060,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>41</v>
       </c>
@@ -10062,7 +10071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>48</v>
       </c>
@@ -10073,7 +10082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>15</v>
       </c>
@@ -10087,7 +10096,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>318</v>
       </c>
@@ -10098,7 +10107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>55</v>
       </c>
@@ -10109,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>12</v>
       </c>
@@ -10120,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>16</v>
       </c>
@@ -10131,7 +10140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>51</v>
       </c>
@@ -10142,7 +10151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>29</v>
       </c>
@@ -10153,7 +10162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>24</v>
       </c>
@@ -10164,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>40</v>
       </c>
@@ -10175,7 +10184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>33</v>
       </c>
@@ -10186,7 +10195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>42</v>
       </c>
@@ -10197,7 +10206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>21</v>
       </c>
@@ -10208,7 +10217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>10</v>
       </c>
@@ -10219,7 +10228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>5</v>
       </c>
@@ -10230,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>36</v>
       </c>
@@ -10241,7 +10250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>315</v>
       </c>
@@ -10252,7 +10261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>30</v>
       </c>
@@ -10263,7 +10272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>320</v>
       </c>
@@ -10274,7 +10283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>56</v>
       </c>
@@ -10285,7 +10294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>22</v>
       </c>
@@ -10296,7 +10305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>13</v>
       </c>
@@ -10307,7 +10316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>46</v>
       </c>
@@ -10318,7 +10327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>25</v>
       </c>
@@ -10329,7 +10338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>44</v>
       </c>
@@ -10340,7 +10349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>311</v>
       </c>
@@ -10351,7 +10360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>59</v>
       </c>
@@ -10362,7 +10371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>35</v>
       </c>
@@ -10373,7 +10382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>317</v>
       </c>
@@ -10384,7 +10393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>45</v>
       </c>
@@ -10395,7 +10404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>38</v>
       </c>
@@ -10406,7 +10415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>316</v>
       </c>
@@ -10417,7 +10426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>7</v>
       </c>
@@ -10428,7 +10437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>18</v>
       </c>
@@ -10439,7 +10448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>57</v>
       </c>
@@ -10450,7 +10459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>60</v>
       </c>
@@ -10461,7 +10470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>32</v>
       </c>
@@ -10472,7 +10481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>17</v>
       </c>
@@ -10483,7 +10492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>50</v>
       </c>
@@ -10494,7 +10503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>26</v>
       </c>
@@ -10505,7 +10514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>19</v>
       </c>
@@ -10516,7 +10525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>49</v>
       </c>
@@ -10527,7 +10536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>34</v>
       </c>
@@ -10538,7 +10547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>319</v>
       </c>
@@ -10552,7 +10561,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>54</v>
       </c>
@@ -10563,7 +10572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>31</v>
       </c>
@@ -10574,7 +10583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>312</v>
       </c>
@@ -10585,7 +10594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>3</v>
       </c>
@@ -10596,7 +10605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>2</v>
       </c>
@@ -10607,7 +10616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>52</v>
       </c>
@@ -10618,7 +10627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>27</v>
       </c>
@@ -10629,7 +10638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>8</v>
       </c>
@@ -10640,7 +10649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>43</v>
       </c>
@@ -10651,7 +10660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>20</v>
       </c>
@@ -10662,7 +10671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>314</v>
       </c>
@@ -10673,7 +10682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>58</v>
       </c>
@@ -10684,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>14</v>
       </c>
@@ -10695,7 +10704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>9</v>
       </c>
@@ -10706,7 +10715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>37</v>
       </c>
@@ -10720,7 +10729,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>47</v>
       </c>
@@ -10731,7 +10740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>39</v>
       </c>
@@ -10742,7 +10751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>313</v>
       </c>
@@ -10753,7 +10762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>28</v>
       </c>
@@ -10764,7 +10773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>53</v>
       </c>
@@ -10775,7 +10784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>23</v>
       </c>
@@ -10786,7 +10795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>182</v>
       </c>
@@ -10800,7 +10809,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>341</v>
       </c>
@@ -10830,9 +10839,9 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>330</v>
       </c>
@@ -10840,7 +10849,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>335</v>
       </c>
@@ -10848,7 +10857,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>336</v>
       </c>
@@ -10856,7 +10865,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>337</v>
       </c>
@@ -10864,7 +10873,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -10872,7 +10881,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>338</v>
       </c>
@@ -10880,7 +10889,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>339</v>
       </c>
@@ -10894,14 +10903,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="51665acc-3f2d-472e-938f-42b3b702aa11">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e03a8b4a-b11d-4666-86ce-dc6b6c932701" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11116,21 +11123,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="51665acc-3f2d-472e-938f-42b3b702aa11">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e03a8b4a-b11d-4666-86ce-dc6b6c932701" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69BC842B-A5E2-4D5A-8170-C24B5F7FBBA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40E094E5-1505-42E3-ACF6-019D70AF5220}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51665acc-3f2d-472e-938f-42b3b702aa11"/>
-    <ds:schemaRef ds:uri="e03a8b4a-b11d-4666-86ce-dc6b6c932701"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11155,9 +11161,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40E094E5-1505-42E3-ACF6-019D70AF5220}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69BC842B-A5E2-4D5A-8170-C24B5F7FBBA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51665acc-3f2d-472e-938f-42b3b702aa11"/>
+    <ds:schemaRef ds:uri="e03a8b4a-b11d-4666-86ce-dc6b6c932701"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>